<commit_message>
Se realizó descripciones de CU del documento Plantilla_de_Casos_de_Uso
</commit_message>
<xml_diff>
--- a/Documents/Plantilla_de_Casos_de_Uso.xlsx
+++ b/Documents/Plantilla_de_Casos_de_Uso.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanGutru\Desktop\SextoSemestre\2.-DesarrolloDeSoftware\PANGEA\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alanglezh/Library/Mobile Documents/com~apple~CloudDocs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4EA8F0-A086-4C20-ADF2-97134309E362}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{61C3994B-72E8-9242-A37F-B3341025DC64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="149">
   <si>
     <t>Columna</t>
   </si>
@@ -173,13 +173,6 @@
     <t>Mostrar eventos</t>
   </si>
   <si>
-    <t>El líder de evento deberá poder crear un evento para gestionar el mismo de manera sencilla.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El lider del evento deberá poder consultar sus eventos en los que se encuentra registrado..
-</t>
-  </si>
-  <si>
     <t>Modificar evento</t>
   </si>
   <si>
@@ -468,6 +461,60 @@
   </si>
   <si>
     <t xml:space="preserve">El miebro de comité deberá poder eliminar el/los material  que ya no se encuentra en condiciones adecuadas para su uso.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Líder Evento deberá poder consultar sus eventos en los que se encuentra registrado..
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Líder Evento deberá poder modificar el evento para actualizar o cambiar su informacón de manera rapida e intuitiva
+</t>
+  </si>
+  <si>
+    <t>El líder Evento  deberá poder crear un evento para gestionar el mismo de manera de manera eficaz.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E Líder Evento deberá poder consultar el programa del evento para poder generarlo en PDF y usarlo fuera del sistema sin complicaciones de formatos. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Líder Comité/Líder Revisor  deberá poder registrar los articulos para que se puedan asignar y revisar de manera segura.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Líder Comité/Líder Revisor  deberá poder modificar los articulos para que se suba una nueva versión de ellos salvaguardando la información.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Líder Comité/Líder Revisor deberá poder asignar un articulo a un revisor para que este pueda evaluarlo y dar retroalimentación de manera intuitiva.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Líder Comité/Líder Revisor deberá poder consultar los articulos que están registrados en el sistema para ver la información de ellos, en un tiempo de repsuesa máximo de 3 segundos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Miembro Comité/Revisor deberá poder crear una revisión del articulos que se le asignó para ofrecer retroalimentación y una evaluación, con la disponibilidad de realizarla en el tiempo que deseé.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Miembro Comité/Revisor deberá poder modificar la revisión que ha dejado pendiente para finalizarla o solo guardarla, estará disponible en todos los casos que aun no sea finalizada. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Líder Comité/Líder Revisor deberá poder enviar la revisión al autor para informarle sobre sus observaciones y calificación, todo en un lapso minimo de máximo de 3 minutos.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La Miembro Comité deberá poder generar las consatancias de los asistentes y ponentes para poder entregarlas por correo electronico de manera intuitiva y eficiente.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Líder Comité/Miembro Comité deberá poder crear una actividad para que su información se encuentre registrada en el sistema y se realicé un seguimiento de ella, en un tiempo máximo de 3 minutos. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Líder Comité/Miembro Comité deberá poder asignar una actividad a su comité especifico para poder llevar el segumiento de los responsables de acividades de manera intuitiva.
 </t>
   </si>
 </sst>
@@ -2043,31 +2090,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="115" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="88.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="1.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="88.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.1640625" style="2" customWidth="1"/>
     <col min="9" max="9" width="49" style="2" customWidth="1"/>
-    <col min="10" max="10" width="39.28515625" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="10.85546875" style="2"/>
+    <col min="10" max="10" width="39.33203125" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:9" ht="37" x14ac:dyDescent="0.45">
       <c r="B1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>15</v>
       </c>
@@ -2075,7 +2122,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" ht="32" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
@@ -2101,18 +2148,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="8" t="s">
         <v>34</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>42</v>
+        <v>137</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>40</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F5" s="6">
         <v>10</v>
@@ -2125,12 +2172,12 @@
       </c>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" ht="32" x14ac:dyDescent="0.2">
       <c r="B6" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>43</v>
+        <v>135</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>41</v>
@@ -2149,15 +2196,15 @@
       </c>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B7" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>8</v>
+        <v>136</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>26</v>
@@ -2173,15 +2220,15 @@
       </c>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B8" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>8</v>
+        <v>138</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>26</v>
@@ -2197,7 +2244,7 @@
       </c>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B9" s="8" t="s">
         <v>38</v>
       </c>
@@ -2205,7 +2252,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>26</v>
@@ -2221,7 +2268,7 @@
       </c>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="2:9" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" s="9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B10" s="12" t="s">
         <v>39</v>
       </c>
@@ -2229,7 +2276,7 @@
         <v>8</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>26</v>
@@ -2245,15 +2292,15 @@
       </c>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>26</v>
@@ -2269,15 +2316,15 @@
       </c>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" ht="64" x14ac:dyDescent="0.2">
       <c r="B12" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>26</v>
@@ -2293,15 +2340,15 @@
       </c>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>8</v>
+        <v>147</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>26</v>
@@ -2317,15 +2364,15 @@
       </c>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>26</v>
@@ -2341,15 +2388,15 @@
       </c>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>26</v>
@@ -2365,15 +2412,15 @@
       </c>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="2:9" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" s="9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B16" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>8</v>
+        <v>148</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>26</v>
@@ -2389,15 +2436,15 @@
       </c>
       <c r="I16" s="11"/>
     </row>
-    <row r="17" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B17" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>26</v>
@@ -2413,15 +2460,15 @@
       </c>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B18" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>26</v>
@@ -2437,15 +2484,15 @@
       </c>
       <c r="I18" s="6"/>
     </row>
-    <row r="19" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B19" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>26</v>
@@ -2461,15 +2508,15 @@
       </c>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B20" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>26</v>
@@ -2485,15 +2532,15 @@
       </c>
       <c r="I20" s="6"/>
     </row>
-    <row r="21" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B21" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>26</v>
@@ -2509,15 +2556,15 @@
       </c>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="2:9" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" s="9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B22" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E22" s="13" t="s">
         <v>26</v>
@@ -2533,15 +2580,15 @@
       </c>
       <c r="I22" s="11"/>
     </row>
-    <row r="23" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B23" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>26</v>
@@ -2557,15 +2604,15 @@
       </c>
       <c r="I23" s="6"/>
     </row>
-    <row r="24" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B24" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>26</v>
@@ -2581,15 +2628,15 @@
       </c>
       <c r="I24" s="6"/>
     </row>
-    <row r="25" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B25" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>26</v>
@@ -2605,15 +2652,15 @@
       </c>
       <c r="I25" s="6"/>
     </row>
-    <row r="26" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B26" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>26</v>
@@ -2629,15 +2676,15 @@
       </c>
       <c r="I26" s="6"/>
     </row>
-    <row r="27" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B27" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>26</v>
@@ -2653,15 +2700,15 @@
       </c>
       <c r="I27" s="6"/>
     </row>
-    <row r="28" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B28" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>26</v>
@@ -2677,15 +2724,15 @@
       </c>
       <c r="I28" s="6"/>
     </row>
-    <row r="29" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B29" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>26</v>
@@ -2701,15 +2748,15 @@
       </c>
       <c r="I29" s="6"/>
     </row>
-    <row r="30" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B30" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>26</v>
@@ -2725,15 +2772,15 @@
       </c>
       <c r="I30" s="6"/>
     </row>
-    <row r="31" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" ht="32" x14ac:dyDescent="0.2">
       <c r="B31" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>26</v>
@@ -2749,15 +2796,15 @@
       </c>
       <c r="I31" s="6"/>
     </row>
-    <row r="32" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B32" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>26</v>
@@ -2773,15 +2820,15 @@
       </c>
       <c r="I32" s="6"/>
     </row>
-    <row r="33" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B33" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>8</v>
+        <v>139</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>26</v>
@@ -2797,15 +2844,15 @@
       </c>
       <c r="I33" s="6"/>
     </row>
-    <row r="34" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B34" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>8</v>
+        <v>140</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>26</v>
@@ -2821,15 +2868,15 @@
       </c>
       <c r="I34" s="6"/>
     </row>
-    <row r="35" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B35" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>8</v>
+        <v>141</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>26</v>
@@ -2845,15 +2892,15 @@
       </c>
       <c r="I35" s="6"/>
     </row>
-    <row r="36" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" ht="32" x14ac:dyDescent="0.2">
       <c r="B36" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>8</v>
+        <v>142</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>26</v>
@@ -2869,15 +2916,15 @@
       </c>
       <c r="I36" s="6"/>
     </row>
-    <row r="37" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B37" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>8</v>
+        <v>143</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>26</v>
@@ -2893,15 +2940,15 @@
       </c>
       <c r="I37" s="6"/>
     </row>
-    <row r="38" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B38" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>8</v>
+        <v>144</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>26</v>
@@ -2917,15 +2964,15 @@
       </c>
       <c r="I38" s="6"/>
     </row>
-    <row r="39" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B39" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>8</v>
+        <v>145</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>26</v>
@@ -2941,7 +2988,7 @@
       </c>
       <c r="I39" s="6"/>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B40" s="8"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
@@ -2951,15 +2998,15 @@
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
     </row>
-    <row r="41" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B41" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>8</v>
+        <v>146</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>26</v>
@@ -2975,15 +3022,15 @@
       </c>
       <c r="I41" s="6"/>
     </row>
-    <row r="42" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B42" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>26</v>
@@ -2999,15 +3046,15 @@
       </c>
       <c r="I42" s="6"/>
     </row>
-    <row r="43" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B43" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>26</v>
@@ -3023,15 +3070,15 @@
       </c>
       <c r="I43" s="6"/>
     </row>
-    <row r="44" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B44" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>26</v>
@@ -3047,15 +3094,15 @@
       </c>
       <c r="I44" s="6"/>
     </row>
-    <row r="45" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B45" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>26</v>
@@ -3071,15 +3118,15 @@
       </c>
       <c r="I45" s="6"/>
     </row>
-    <row r="46" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B46" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>26</v>
@@ -3095,15 +3142,15 @@
       </c>
       <c r="I46" s="6"/>
     </row>
-    <row r="47" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B47" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>26</v>
@@ -3119,15 +3166,15 @@
       </c>
       <c r="I47" s="6"/>
     </row>
-    <row r="48" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B48" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>26</v>
@@ -3143,7 +3190,7 @@
       </c>
       <c r="I48" s="6"/>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B49" s="8"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
@@ -3153,7 +3200,7 @@
       <c r="H49" s="6"/>
       <c r="I49" s="6"/>
     </row>
-    <row r="50" spans="2:9" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:9" s="9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B50" s="10" t="s">
         <v>7</v>
       </c>
@@ -3581,26 +3628,26 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.42578125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="1.5" style="5" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" style="5" customWidth="1"/>
     <col min="3" max="3" width="86" style="5" customWidth="1"/>
-    <col min="4" max="4" width="2.85546875" style="5" customWidth="1"/>
-    <col min="5" max="16384" width="10.85546875" style="5"/>
+    <col min="4" max="4" width="2.83203125" style="5" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:9" ht="37" x14ac:dyDescent="0.45">
       <c r="B1" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -3608,7 +3655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
@@ -3616,7 +3663,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" ht="80" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
@@ -3624,7 +3671,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" ht="48" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
         <v>5</v>
       </c>
@@ -3632,7 +3679,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="210" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" ht="192" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
         <v>2</v>
       </c>
@@ -3655,7 +3702,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
         <v>22</v>
       </c>
@@ -3663,7 +3710,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" ht="32" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
         <v>19</v>
       </c>
@@ -3671,7 +3718,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" ht="32" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
         <v>3</v>
       </c>
@@ -3688,7 +3735,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" ht="32" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
actualización de plantilla de casos de uso
</commit_message>
<xml_diff>
--- a/Documents/Plantilla_de_Casos_de_Uso.xlsx
+++ b/Documents/Plantilla_de_Casos_de_Uso.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vik-t\Documents\SoftwareEngineering\6toSemestre\DesarrolloDeSoftware\PANGEA\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395350F9-492D-42E1-A047-2F81C6481CAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1620C7F5-8521-404F-AF57-DA88089370B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="158">
   <si>
     <t>Columna</t>
   </si>
@@ -545,6 +545,14 @@
   </si>
   <si>
     <t xml:space="preserve">El líder del evento deberá poder eliminar personal del evento para poder tener control de quienes ya no participan en el evento  esto de manera sencilla e intuitiva.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El líder de evento deberá poder crear un comité para poder llevar el control de los organizadores de manera fácil e intuitiva.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El líder de evento y comité deberá poder modificar los miembros del comité con el fin de agregar o elimianar miembros de manera sencilla e intuitiva.
 </t>
   </si>
 </sst>
@@ -2120,8 +2128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29:D48"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="91" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2279,7 +2287,7 @@
         <v>38</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>8</v>
+        <v>156</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>44</v>
@@ -2288,7 +2296,7 @@
         <v>26</v>
       </c>
       <c r="F9" s="6">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G9" s="6">
         <v>1</v>
@@ -2303,7 +2311,7 @@
         <v>39</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>8</v>
+        <v>157</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>45</v>
@@ -2312,7 +2320,7 @@
         <v>26</v>
       </c>
       <c r="F10" s="6">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G10" s="6">
         <v>1</v>
@@ -2336,7 +2344,7 @@
         <v>26</v>
       </c>
       <c r="F11" s="6">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G11" s="6">
         <v>1</v>
@@ -2360,7 +2368,7 @@
         <v>26</v>
       </c>
       <c r="F12" s="6">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G12" s="6">
         <v>1</v>
@@ -2480,7 +2488,7 @@
         <v>26</v>
       </c>
       <c r="F17" s="6">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G17" s="6">
         <v>1</v>
@@ -2528,7 +2536,7 @@
         <v>26</v>
       </c>
       <c r="F19" s="6">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G19" s="6">
         <v>1</v>
@@ -3654,8 +3662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:I12"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="B1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Menu principal para pangea, diagramas de secuencia de CU05
</commit_message>
<xml_diff>
--- a/Documents/Plantilla_de_Casos_de_Uso.xlsx
+++ b/Documents/Plantilla_de_Casos_de_Uso.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vik-t\Documents\SoftwareEngineering\6toSemestre\DesarrolloDeSoftware\PANGEA\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1620C7F5-8521-404F-AF57-DA88089370B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1FC450-1A06-4484-BD85-4FF284C223C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="159">
   <si>
     <t>Columna</t>
   </si>
@@ -553,6 +553,10 @@
   </si>
   <si>
     <t xml:space="preserve">El líder de evento y comité deberá poder modificar los miembros del comité con el fin de agregar o elimianar miembros de manera sencilla e intuitiva.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El líder evento y líder comité deberá poder modificar la información del comité para actulizar los datos.
 </t>
   </si>
 </sst>
@@ -2128,8 +2132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="91" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="91" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2286,7 +2290,7 @@
       <c r="B9" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="13" t="s">
         <v>156</v>
       </c>
       <c r="D9" s="6" t="s">
@@ -2335,7 +2339,7 @@
         <v>47</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>8</v>
+        <v>158</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>46</v>

</xml_diff>